<commit_message>
La till en till testfil med mer vanliga meningar + testdata.
</commit_message>
<xml_diff>
--- a/Testreultat.xlsx
+++ b/Testreultat.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Ngram</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>% rätt</t>
+  </si>
+  <si>
+    <t>Enkla meningar "easy:english:sentences.txt"</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -104,12 +113,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -400,13 +409,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -429,16 +438,16 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>46060</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>37404</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>8656</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E6" si="0">C3/B3</f>
         <v>0.81207121146330874</v>
       </c>
@@ -447,16 +456,16 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>46060</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>35881</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>10179</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>0.77900564481111589</v>
       </c>
@@ -465,16 +474,16 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>46060</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>35907</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>10153</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>0.77957012592270947</v>
       </c>
@@ -483,16 +492,16 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>46060</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>35907</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>10153</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.77957012592270947</v>
       </c>
@@ -501,28 +510,28 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>46060</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>35907</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>10153</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f>C7/B7</f>
         <v>0.77957012592270947</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -545,16 +554,16 @@
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>6655</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>5118</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>1537</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f>C12/B12</f>
         <v>0.769045830202855</v>
       </c>
@@ -563,16 +572,16 @@
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>6655</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>4943</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>1712</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <f t="shared" ref="E13:E16" si="1">C13/B13</f>
         <v>0.74274981217129976</v>
       </c>
@@ -581,16 +590,16 @@
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>6655</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>4945</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>1710</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" si="1"/>
         <v>0.74305033809166043</v>
       </c>
@@ -599,16 +608,16 @@
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>6655</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>4945</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>1710</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f t="shared" si="1"/>
         <v>0.74305033809166043</v>
       </c>
@@ -617,24 +626,146 @@
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>6655</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>4945</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>1710</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f t="shared" si="1"/>
         <v>0.74305033809166043</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4784034</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4097538</v>
+      </c>
+      <c r="D20" s="1">
+        <v>686496</v>
+      </c>
+      <c r="E20" s="2">
+        <f>C20/B20</f>
+        <v>0.85650269207952956</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4784034</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3921207</v>
+      </c>
+      <c r="D21" s="1">
+        <v>862827</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" ref="E21:E24" si="2">C21/B21</f>
+        <v>0.81964446740972163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4784034</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3921884</v>
+      </c>
+      <c r="D22" s="1">
+        <v>862150</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.81978597978191625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4784034</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3921868</v>
+      </c>
+      <c r="D23" s="1">
+        <v>862166</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.81978263532408002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Har gjort om ordlistan så att alla ord i t9 är samma som i 1-gram. Ny testfil med 9000 ord.
</commit_message>
<xml_diff>
--- a/Testreultat.xlsx
+++ b/Testreultat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -119,6 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +401,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E21" sqref="E21:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,7 +698,7 @@
       <c r="D21" s="1">
         <v>862827</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="5">
         <f t="shared" ref="E21:E24" si="2">C21/B21</f>
         <v>0.81964446740972163</v>
       </c>
@@ -715,7 +716,7 @@
       <c r="D22" s="1">
         <v>862150</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="5">
         <f t="shared" si="2"/>
         <v>0.81978597978191625</v>
       </c>
@@ -733,7 +734,7 @@
       <c r="D23" s="1">
         <v>862166</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="5">
         <f t="shared" si="2"/>
         <v>0.81978263532408002</v>
       </c>

</xml_diff>